<commit_message>
corrected data file error, updated analyses and preprint
</commit_message>
<xml_diff>
--- a/data/data existence and availability.xlsx
+++ b/data/data existence and availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/repository-of-published-irap-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4669CC51-1D8C-574C-9009-70DE92ECB0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D6EAB2-F2D7-5147-8114-6C3FAD72BB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32780" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1492,7 +1492,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1511,9 +1511,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1873,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F9036-BD7F-8941-AAC0-FD3B8EC13872}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="119" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="119" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="topRight" activeCell="L42" sqref="L42"/>
     </sheetView>
@@ -3279,7 +3276,7 @@
       <c r="K38" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="L38" s="8"/>
+      <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">

</xml_diff>